<commit_message>
Added pdf and png versions, updated Ops FMEA
</commit_message>
<xml_diff>
--- a/FMEA_Application.xlsx
+++ b/FMEA_Application.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anc/WorkDocs/Thought Leading/Resilience/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DA3A75-D93E-5B48-BD80-FC9869660ADB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83E74A3-B02F-7446-A5AB-06B1F1F958E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,10 @@
     <sheet name="Probability" sheetId="4" r:id="rId3"/>
     <sheet name="Detectability" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">FMEA!$A$1:$P$28</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -1432,11 +1435,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="172" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="E1" sqref="E1:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1551,7 +1555,7 @@
       </c>
       <c r="M4" s="101">
         <f ca="1">NOW()</f>
-        <v>43531.963892939813</v>
+        <v>43779.980831018518</v>
       </c>
       <c r="N4" s="102"/>
       <c r="O4" s="102"/>
@@ -2328,6 +2332,7 @@
     <mergeCell ref="E1:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="57" fitToHeight="3" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>